<commit_message>
hago variable la busqueda del archivo excel de Menta de entrada segun el parametro fecha de proceso que recibo en procesador.php
</commit_message>
<xml_diff>
--- a/archivocuotas.xlsx
+++ b/archivocuotas.xlsx
@@ -378,8 +378,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <f>RANDBETWEEN(11111111,99999999)</f>
-        <v>12276464</v>
+        <v>1818072874.0</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -387,8 +386,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <f>RANDBETWEEN(11111111,99999999)</f>
-        <v>53714619</v>
+        <v>1822225502.0</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -396,8 +394,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <f>RANDBETWEEN(11111111,99999999)</f>
-        <v>13951410</v>
+        <v>1195849953.0</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -405,8 +402,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <f>RANDBETWEEN(11111111,99999999)</f>
-        <v>47705445</v>
+        <v>1206482622.0</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -414,8 +410,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <f>RANDBETWEEN(11111111,99999999)</f>
-        <v>58322165</v>
+        <v>1155066173.0</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -423,8 +418,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <f>RANDBETWEEN(11111111,99999999)</f>
-        <v>36600871</v>
+        <v>1547902419.0</v>
       </c>
       <c r="B7">
         <v>6</v>

</xml_diff>